<commit_message>
tested t5-small locally: everything works
</commit_message>
<xml_diff>
--- a/data/human_annotation/ELINsample_for_check_human.xlsx
+++ b/data/human_annotation/ELINsample_for_check_human.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/xnauel$/Göteborg 2014-2021/RJ mIxed methods/fatherhood paper from jan 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llupo/dev/pappa/data/human_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D42756D4-DF19-BF42-8CDA-0699BB20144F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3D6CFD-46CD-7145-8272-29E9CF569058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="to code" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="labels" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1942,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B344" sqref="B344"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>